<commit_message>
Added column to distinguish plugs
</commit_message>
<xml_diff>
--- a/tree_ghg/GCREW_TreeGas_01_23_2019.xlsx
+++ b/tree_ghg/GCREW_TreeGas_01_23_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penn529\Documents\Github\PREMIS-ghg\tree_ghg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8BEBD8F-996B-480A-8529-5067A234B102}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C05D0F6-58D4-4E06-8AAD-93222510DF44}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{A0BB915F-05FE-134D-9CE0-852DFBE336D7}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>negative pressure - needle sucked in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plug Height </t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
@@ -626,55 +632,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{022806E5-818B-1A45-B771-EFD8981A779B}">
-  <dimension ref="A1:AC24"/>
+  <dimension ref="A1:AD24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.69921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.69921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.69921875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.69921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>45</v>
       </c>
-      <c r="O1">
-        <f>M4*200</f>
+      <c r="P1">
+        <f>N4*200</f>
         <v>8400</v>
       </c>
-      <c r="Q1">
-        <f>M4*0.5</f>
+      <c r="R1">
+        <f>N4*0.5</f>
         <v>21</v>
       </c>
-      <c r="S1">
-        <f>0.3*M4</f>
+      <c r="T1">
+        <f>0.3*N4</f>
         <v>12.6</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -694,70 +700,73 @@
         <v>29</v>
       </c>
       <c r="G3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="N3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="P3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="Q3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="R3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="T3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="U3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="V3" s="9" t="s">
+      <c r="W3" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="X3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="Y3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="Y3" s="9" t="s">
+      <c r="Z3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="Z3" s="9" t="s">
+      <c r="AA3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="AA3" s="9" t="s">
+      <c r="AB3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AB3" s="9" t="s">
+      <c r="AC3" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AC3" s="9" t="s">
+      <c r="AD3" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>43488</v>
       </c>
@@ -776,33 +785,32 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="H4">
-        <v>12</v>
+      <c r="G4" t="s">
+        <v>71</v>
       </c>
       <c r="I4">
-        <f>(H4+F4)/F4</f>
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <f>(I4+F4)/F4</f>
         <v>7</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>10</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>50</v>
       </c>
-      <c r="L4">
-        <f>(K4+J4)/J4</f>
+      <c r="M4">
+        <f>(L4+K4)/K4</f>
         <v>6</v>
       </c>
-      <c r="M4">
-        <f>I4*L4</f>
+      <c r="N4">
+        <f>J4*M4</f>
         <v>42</v>
       </c>
-      <c r="X4">
-        <f t="shared" ref="X4:AC4" si="0">O4*$M4</f>
-        <v>0</v>
-      </c>
       <c r="Y4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Y4:AD4" si="0">P4*$N4</f>
         <v>0</v>
       </c>
       <c r="Z4">
@@ -821,8 +829,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AD4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>43488</v>
       </c>
@@ -841,33 +853,32 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="H5">
-        <v>12</v>
+      <c r="G5" t="s">
+        <v>71</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I24" si="1">(H5+F5)/F5</f>
+        <v>12</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J24" si="1">(I5+F5)/F5</f>
         <v>7</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>10</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>50</v>
       </c>
-      <c r="L5">
-        <f>(K5+J5)/J5</f>
+      <c r="M5">
+        <f>(L5+K5)/K5</f>
         <v>6</v>
       </c>
-      <c r="M5">
-        <f>I5*L5</f>
+      <c r="N5">
+        <f>J5*M5</f>
         <v>42</v>
       </c>
-      <c r="X5">
-        <f t="shared" ref="X5:AC24" si="2">O5*$M5</f>
-        <v>0</v>
-      </c>
       <c r="Y5">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="Y5:AD24" si="2">P5*$N5</f>
         <v>0</v>
       </c>
       <c r="Z5">
@@ -886,8 +897,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>43488</v>
       </c>
@@ -906,31 +921,30 @@
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="H6">
-        <v>12</v>
+      <c r="G6" t="s">
+        <v>71</v>
       </c>
       <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>10</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>50</v>
       </c>
-      <c r="L6">
-        <f t="shared" ref="L6:L24" si="3">(K6+J6)/J6</f>
+      <c r="M6">
+        <f t="shared" ref="M6:M24" si="3">(L6+K6)/K6</f>
         <v>6</v>
       </c>
-      <c r="M6">
-        <f t="shared" ref="M6:M24" si="4">I6*L6</f>
+      <c r="N6">
+        <f t="shared" ref="N6:N24" si="4">J6*M6</f>
         <v>42</v>
       </c>
-      <c r="X6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -951,8 +965,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>43488</v>
       </c>
@@ -971,31 +989,30 @@
       <c r="F7">
         <v>2</v>
       </c>
-      <c r="H7">
-        <v>12</v>
+      <c r="G7" t="s">
+        <v>71</v>
       </c>
       <c r="I7">
+        <v>12</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>10</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>50</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="X7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y7">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1016,8 +1033,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>43488</v>
       </c>
@@ -1036,31 +1057,30 @@
       <c r="F8">
         <v>2</v>
       </c>
-      <c r="H8">
-        <v>12</v>
+      <c r="G8" t="s">
+        <v>71</v>
       </c>
       <c r="I8">
+        <v>12</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>10</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>50</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="X8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y8">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1081,8 +1101,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>43488</v>
       </c>
@@ -1101,31 +1125,30 @@
       <c r="F9">
         <v>2</v>
       </c>
-      <c r="H9">
-        <v>12</v>
+      <c r="G9" t="s">
+        <v>71</v>
       </c>
       <c r="I9">
+        <v>12</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>10</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>50</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="X9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y9">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1146,8 +1169,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>43488</v>
       </c>
@@ -1166,31 +1193,30 @@
       <c r="F10" s="4">
         <v>2</v>
       </c>
-      <c r="H10" s="4">
-        <v>12</v>
+      <c r="G10" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="I10" s="4">
+        <v>12</v>
+      </c>
+      <c r="J10" s="4">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J10" s="4">
+      <c r="K10" s="4">
         <v>10</v>
       </c>
-      <c r="K10" s="4">
+      <c r="L10" s="4">
         <v>50</v>
       </c>
-      <c r="L10" s="4">
+      <c r="M10" s="4">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M10" s="4">
+      <c r="N10" s="4">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="X10" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y10" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1211,8 +1237,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD10" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>43488</v>
       </c>
@@ -1231,31 +1261,30 @@
       <c r="F11" s="4">
         <v>2</v>
       </c>
-      <c r="H11" s="4">
-        <v>12</v>
+      <c r="G11" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="I11" s="4">
+        <v>12</v>
+      </c>
+      <c r="J11" s="4">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J11" s="4">
+      <c r="K11" s="4">
         <v>10</v>
       </c>
-      <c r="K11" s="4">
+      <c r="L11" s="4">
         <v>50</v>
       </c>
-      <c r="L11" s="4">
+      <c r="M11" s="4">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M11" s="4">
+      <c r="N11" s="4">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="X11" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y11" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1276,8 +1305,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD11" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>43488</v>
       </c>
@@ -1296,31 +1329,30 @@
       <c r="F12" s="4">
         <v>1.8</v>
       </c>
-      <c r="H12" s="4">
-        <v>12</v>
+      <c r="G12" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="I12" s="4">
+        <v>12</v>
+      </c>
+      <c r="J12" s="4">
         <f t="shared" si="1"/>
         <v>7.666666666666667</v>
       </c>
-      <c r="J12" s="4">
+      <c r="K12" s="4">
         <v>10</v>
       </c>
-      <c r="K12" s="4">
+      <c r="L12" s="4">
         <v>50</v>
       </c>
-      <c r="L12" s="4">
+      <c r="M12" s="4">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M12" s="4">
+      <c r="N12" s="4">
         <f t="shared" si="4"/>
         <v>46</v>
       </c>
-      <c r="X12" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y12" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1341,8 +1373,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD12" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>43488</v>
       </c>
@@ -1361,31 +1397,30 @@
       <c r="F13" s="4">
         <v>2</v>
       </c>
-      <c r="H13" s="4">
-        <v>12</v>
+      <c r="G13" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="I13" s="4">
+        <v>12</v>
+      </c>
+      <c r="J13" s="4">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J13" s="4">
+      <c r="K13" s="4">
         <v>10</v>
       </c>
-      <c r="K13" s="4">
+      <c r="L13" s="4">
         <v>50</v>
       </c>
-      <c r="L13" s="4">
+      <c r="M13" s="4">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M13" s="4">
+      <c r="N13" s="4">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="X13" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y13" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1406,8 +1441,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD13" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>43488</v>
       </c>
@@ -1426,31 +1465,30 @@
       <c r="F14" s="4">
         <v>2</v>
       </c>
-      <c r="H14" s="4">
-        <v>12</v>
+      <c r="G14" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="I14" s="4">
+        <v>12</v>
+      </c>
+      <c r="J14" s="4">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J14" s="4">
+      <c r="K14" s="4">
         <v>10</v>
       </c>
-      <c r="K14" s="4">
+      <c r="L14" s="4">
         <v>50</v>
       </c>
-      <c r="L14" s="4">
+      <c r="M14" s="4">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M14" s="4">
+      <c r="N14" s="4">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="X14" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y14" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1471,8 +1509,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD14" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>43488</v>
       </c>
@@ -1491,31 +1533,30 @@
       <c r="F15" s="6">
         <v>2</v>
       </c>
-      <c r="H15" s="6">
-        <v>12</v>
+      <c r="G15" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="I15" s="6">
-        <f>(H15+F15)/F15</f>
+        <v>12</v>
+      </c>
+      <c r="J15" s="6">
+        <f>(I15+F15)/F15</f>
         <v>7</v>
       </c>
-      <c r="J15" s="6">
+      <c r="K15" s="6">
         <v>10</v>
       </c>
-      <c r="K15" s="6">
+      <c r="L15" s="6">
         <v>50</v>
       </c>
-      <c r="L15" s="6">
-        <f>(K15+J15)/J15</f>
+      <c r="M15" s="6">
+        <f>(L15+K15)/K15</f>
         <v>6</v>
       </c>
-      <c r="M15" s="6">
-        <f>I15*L15</f>
+      <c r="N15" s="6">
+        <f>J15*M15</f>
         <v>42</v>
       </c>
-      <c r="X15" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y15" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1536,8 +1577,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD15" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>43488</v>
       </c>
@@ -1556,31 +1601,30 @@
       <c r="F16" s="6">
         <v>1.8</v>
       </c>
-      <c r="H16" s="6">
-        <v>12</v>
+      <c r="G16" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="I16" s="6">
-        <f>(H16+F16)/F16</f>
+        <v>12</v>
+      </c>
+      <c r="J16" s="6">
+        <f>(I16+F16)/F16</f>
         <v>7.666666666666667</v>
       </c>
-      <c r="J16" s="6">
+      <c r="K16" s="6">
         <v>10</v>
       </c>
-      <c r="K16" s="6">
+      <c r="L16" s="6">
         <v>50</v>
       </c>
-      <c r="L16" s="6">
-        <f>(K16+J16)/J16</f>
+      <c r="M16" s="6">
+        <f>(L16+K16)/K16</f>
         <v>6</v>
       </c>
-      <c r="M16" s="6">
-        <f>I16*L16</f>
+      <c r="N16" s="6">
+        <f>J16*M16</f>
         <v>46</v>
       </c>
-      <c r="X16" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y16" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1601,8 +1645,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD16" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>43488</v>
       </c>
@@ -1622,33 +1670,32 @@
         <v>2</v>
       </c>
       <c r="G17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="6">
-        <v>12</v>
-      </c>
       <c r="I17" s="6">
-        <f>(H17+F17)/F17</f>
+        <v>12</v>
+      </c>
+      <c r="J17" s="6">
+        <f>(I17+F17)/F17</f>
         <v>7</v>
       </c>
-      <c r="J17" s="6">
+      <c r="K17" s="6">
         <v>10</v>
       </c>
-      <c r="K17" s="6">
+      <c r="L17" s="6">
         <v>50</v>
       </c>
-      <c r="L17" s="6">
-        <f>(K17+J17)/J17</f>
+      <c r="M17" s="6">
+        <f>(L17+K17)/K17</f>
         <v>6</v>
       </c>
-      <c r="M17" s="6">
-        <f>I17*L17</f>
+      <c r="N17" s="6">
+        <f>J17*M17</f>
         <v>42</v>
       </c>
-      <c r="X17" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y17" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1669,8 +1716,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD17" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>43488</v>
       </c>
@@ -1689,31 +1740,30 @@
       <c r="F18" s="6">
         <v>2</v>
       </c>
-      <c r="H18" s="6">
-        <v>12</v>
+      <c r="G18" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="I18" s="6">
-        <f>(H18+F18)/F18</f>
+        <v>12</v>
+      </c>
+      <c r="J18" s="6">
+        <f>(I18+F18)/F18</f>
         <v>7</v>
       </c>
-      <c r="J18" s="6">
+      <c r="K18" s="6">
         <v>10</v>
       </c>
-      <c r="K18" s="6">
+      <c r="L18" s="6">
         <v>50</v>
       </c>
-      <c r="L18" s="6">
-        <f>(K18+J18)/J18</f>
+      <c r="M18" s="6">
+        <f>(L18+K18)/K18</f>
         <v>6</v>
       </c>
-      <c r="M18" s="6">
-        <f>I18*L18</f>
+      <c r="N18" s="6">
+        <f>J18*M18</f>
         <v>42</v>
       </c>
-      <c r="X18" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y18" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1734,8 +1784,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD18" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>43488</v>
       </c>
@@ -1754,31 +1808,30 @@
       <c r="F19" s="6">
         <v>2</v>
       </c>
-      <c r="H19" s="6">
-        <v>12</v>
+      <c r="G19" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="I19" s="6">
-        <f>(H19+F19)/F19</f>
+        <v>12</v>
+      </c>
+      <c r="J19" s="6">
+        <f>(I19+F19)/F19</f>
         <v>7</v>
       </c>
-      <c r="J19" s="6">
+      <c r="K19" s="6">
         <v>10</v>
       </c>
-      <c r="K19" s="6">
+      <c r="L19" s="6">
         <v>50</v>
       </c>
-      <c r="L19" s="6">
-        <f>(K19+J19)/J19</f>
+      <c r="M19" s="6">
+        <f>(L19+K19)/K19</f>
         <v>6</v>
       </c>
-      <c r="M19" s="6">
-        <f>I19*L19</f>
+      <c r="N19" s="6">
+        <f>J19*M19</f>
         <v>42</v>
       </c>
-      <c r="X19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y19" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1799,8 +1852,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD19" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>43488</v>
       </c>
@@ -1819,31 +1876,30 @@
       <c r="F20" s="8">
         <v>2</v>
       </c>
-      <c r="H20" s="8">
-        <v>12</v>
+      <c r="G20" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="I20" s="8">
+        <v>12</v>
+      </c>
+      <c r="J20" s="8">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J20" s="8">
+      <c r="K20" s="8">
         <v>10</v>
       </c>
-      <c r="K20" s="8">
+      <c r="L20" s="8">
         <v>50</v>
       </c>
-      <c r="L20" s="8">
+      <c r="M20" s="8">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M20" s="8">
+      <c r="N20" s="8">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="X20" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y20" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1864,8 +1920,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD20" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>43488</v>
       </c>
@@ -1884,31 +1944,30 @@
       <c r="F21" s="8">
         <v>2</v>
       </c>
-      <c r="H21" s="8">
-        <v>12</v>
+      <c r="G21" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="I21" s="8">
+        <v>12</v>
+      </c>
+      <c r="J21" s="8">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J21" s="8">
+      <c r="K21" s="8">
         <v>10</v>
       </c>
-      <c r="K21" s="8">
+      <c r="L21" s="8">
         <v>50</v>
       </c>
-      <c r="L21" s="8">
+      <c r="M21" s="8">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M21" s="8">
+      <c r="N21" s="8">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="X21" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y21" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1929,8 +1988,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD21" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>43488</v>
       </c>
@@ -1949,31 +2012,30 @@
       <c r="F22" s="8">
         <v>2</v>
       </c>
-      <c r="H22" s="8">
-        <v>12</v>
+      <c r="G22" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="I22" s="8">
+        <v>12</v>
+      </c>
+      <c r="J22" s="8">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J22" s="8">
+      <c r="K22" s="8">
         <v>10</v>
       </c>
-      <c r="K22" s="8">
+      <c r="L22" s="8">
         <v>50</v>
       </c>
-      <c r="L22" s="8">
+      <c r="M22" s="8">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M22" s="8">
+      <c r="N22" s="8">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="X22" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y22" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1994,8 +2056,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD22" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>43488</v>
       </c>
@@ -2014,31 +2080,30 @@
       <c r="F23" s="8">
         <v>2</v>
       </c>
-      <c r="H23" s="8">
-        <v>12</v>
+      <c r="G23" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="I23" s="8">
+        <v>12</v>
+      </c>
+      <c r="J23" s="8">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J23" s="8">
+      <c r="K23" s="8">
         <v>10</v>
       </c>
-      <c r="K23" s="8">
+      <c r="L23" s="8">
         <v>50</v>
       </c>
-      <c r="L23" s="8">
+      <c r="M23" s="8">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M23" s="8">
+      <c r="N23" s="8">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="X23" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y23" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2059,8 +2124,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="AD23" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>43488</v>
       </c>
@@ -2080,33 +2149,32 @@
         <v>2</v>
       </c>
       <c r="G24" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H24" s="8">
-        <v>12</v>
-      </c>
       <c r="I24" s="8">
+        <v>12</v>
+      </c>
+      <c r="J24" s="8">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J24" s="8">
+      <c r="K24" s="8">
         <v>10</v>
       </c>
-      <c r="K24" s="8">
+      <c r="L24" s="8">
         <v>50</v>
       </c>
-      <c r="L24" s="8">
+      <c r="M24" s="8">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M24" s="8">
+      <c r="N24" s="8">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="X24" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="Y24" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2124,6 +2192,10 @@
         <v>0</v>
       </c>
       <c r="AC24" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AD24" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>

</xml_diff>